<commit_message>
adding revised analyses, these will greatly be reduced upon resbumission of manuscript
</commit_message>
<xml_diff>
--- a/3D Modeling/data/3D Model Surface Areas.xlsx
+++ b/3D Modeling/data/3D Model Surface Areas.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iancombs/Documents/GitHub/analysisOf3dModels/3D Modeling/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0146B609-29EB-E040-A696-E2814F57BE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="33600" windowHeight="19260" xr2:uid="{955A6041-912B-9A46-9DD3-482E54DADD3F}"/>
+    <workbookView xWindow="0" yWindow="975" windowWidth="22890" windowHeight="8415" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="8.24.18" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Proportion" sheetId="5" r:id="rId6"/>
     <sheet name="Rates of Change" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -431,7 +425,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
     <numFmt numFmtId="165" formatCode="0.000000000000000"/>
@@ -805,40 +799,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39FF2E5-D6B1-4546-9458-72DB78A9AD32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T2" sqref="T2:U32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="43.375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -870,7 +864,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -906,7 +900,7 @@
         <v>3.3080277699999998E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -944,7 +938,7 @@
       <c r="W3"/>
       <c r="X3"/>
     </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -970,7 +964,7 @@
       <c r="W4"/>
       <c r="X4"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1000,7 @@
         <v>3.5793772700000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1039,7 +1033,7 @@
         <v>3.35460796E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1095,7 @@
       <c r="W7"/>
       <c r="X7"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1144,7 @@
       </c>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1171,7 +1165,7 @@
       <c r="W9"/>
       <c r="X9"/>
     </row>
-    <row r="10" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1206,7 +1200,7 @@
       <c r="W10"/>
       <c r="X10"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1242,7 +1236,7 @@
         <v>4.6742823600000004E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1267,7 +1261,7 @@
       </c>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1314,7 +1308,7 @@
       <c r="W13"/>
       <c r="X13"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1353,7 +1347,7 @@
         <v>3.47565257E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1374,7 +1368,7 @@
         <v>3.3644091000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1401,7 +1395,7 @@
         <v>3.1354793200000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1428,7 +1422,7 @@
         <v>3.0993404900000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1452,7 +1446,7 @@
         <v>3.3425866199999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1479,7 +1473,7 @@
         <v>3.06581672E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1527,7 +1521,7 @@
         <v>3.29427254E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1584,7 +1578,7 @@
         <v>3.7530946700000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1617,7 @@
         <v>3.0481838100000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1647,7 +1641,7 @@
         <v>3.38797383E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1686,7 +1680,7 @@
         <v>3.28589892E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1707,7 +1701,7 @@
         <v>3.3924032800000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1731,7 +1725,7 @@
         <v>3.16762486E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1779,7 +1773,7 @@
         <v>3.79125377E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>3.7355130899999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1830,7 +1824,7 @@
         <v>3.6922170999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1881,7 +1875,7 @@
         <v>3.5980866599999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1914,7 +1908,7 @@
         <v>3.25294776E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1983,7 +1977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24144803-0D0C-114E-A859-9A12269B7D2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
@@ -1991,18 +1985,18 @@
       <selection pane="topRight" activeCell="AA21" sqref="AA21:AB33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="8" customWidth="1"/>
-    <col min="3" max="25" width="14.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.375" style="8" customWidth="1"/>
+    <col min="3" max="25" width="14.625" style="8" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="8"/>
+    <col min="27" max="27" width="15.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -2025,7 +2019,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -2051,7 +2045,7 @@
       <c r="AD2"/>
       <c r="AE2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -2080,7 +2074,7 @@
       <c r="AD3"/>
       <c r="AE3"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -2110,7 +2104,7 @@
       <c r="AD4"/>
       <c r="AE4"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -2148,7 +2142,7 @@
       <c r="AD5"/>
       <c r="AE5"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -2174,7 +2168,7 @@
       <c r="AD6"/>
       <c r="AE6"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -2221,7 +2215,7 @@
       <c r="AD7"/>
       <c r="AE7"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -2268,7 +2262,7 @@
       <c r="AD8"/>
       <c r="AE8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2289,7 @@
       <c r="AD9"/>
       <c r="AE9"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2333,7 +2327,7 @@
       <c r="AD10"/>
       <c r="AE10"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
@@ -2362,7 +2356,7 @@
       <c r="AD11"/>
       <c r="AE11"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -2394,7 +2388,7 @@
       <c r="AD12"/>
       <c r="AE12"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -2462,7 +2456,7 @@
       <c r="AD13"/>
       <c r="AE13"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2507,7 +2501,7 @@
       <c r="AD14"/>
       <c r="AE14"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
@@ -2545,7 +2539,7 @@
       <c r="AD15"/>
       <c r="AE15"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -2580,7 +2574,7 @@
       <c r="AD16"/>
       <c r="AE16"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
@@ -2604,7 +2598,7 @@
       <c r="AD17"/>
       <c r="AE17"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -2636,7 +2630,7 @@
       <c r="AD18"/>
       <c r="AE18"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -2662,7 +2656,7 @@
       <c r="AD19"/>
       <c r="AE19"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>39</v>
       </c>
@@ -2684,7 +2678,7 @@
       <c r="AD20"/>
       <c r="AE20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -2737,7 +2731,7 @@
       <c r="AD21"/>
       <c r="AE21"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
@@ -2802,7 +2796,7 @@
       <c r="AD22"/>
       <c r="AE22"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
@@ -2855,7 +2849,7 @@
       <c r="AD23"/>
       <c r="AE23"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
@@ -2893,7 +2887,7 @@
       <c r="AD24"/>
       <c r="AE24"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>25</v>
       </c>
@@ -2958,7 +2952,7 @@
       <c r="AD25"/>
       <c r="AE25"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>26</v>
       </c>
@@ -2984,7 +2978,7 @@
       <c r="AD26"/>
       <c r="AE26"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>27</v>
       </c>
@@ -3019,7 +3013,7 @@
       <c r="AD27"/>
       <c r="AE27"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
@@ -3078,7 +3072,7 @@
       <c r="AD28"/>
       <c r="AE28"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
@@ -3116,7 +3110,7 @@
       <c r="AD29"/>
       <c r="AE29"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>29</v>
       </c>
@@ -3148,7 +3142,7 @@
       <c r="AD30"/>
       <c r="AE30"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>30</v>
       </c>
@@ -3204,7 +3198,7 @@
       <c r="AD31"/>
       <c r="AE31"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>31</v>
       </c>
@@ -3293,7 +3287,7 @@
       <c r="AD32"/>
       <c r="AE32"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>32</v>
       </c>
@@ -3382,7 +3376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74316578-E42F-554F-90BF-6D57C7835EEA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3390,19 +3384,19 @@
       <selection pane="topRight" activeCell="AA21" sqref="AA21:AB33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.33203125" style="3" customWidth="1"/>
-    <col min="4" max="21" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="9.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.375" style="3" customWidth="1"/>
+    <col min="4" max="21" width="12.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="10.875" style="3"/>
     <col min="26" max="26" width="22.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="3"/>
+    <col min="27" max="27" width="15.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3425,7 +3419,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -3457,7 +3451,7 @@
       <c r="AD2"/>
       <c r="AE2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3486,7 +3480,7 @@
       <c r="AD3"/>
       <c r="AE3"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -3516,7 +3510,7 @@
       <c r="AD4"/>
       <c r="AE4"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -3551,7 +3545,7 @@
       <c r="AD5"/>
       <c r="AE5"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3577,7 +3571,7 @@
       <c r="AD6"/>
       <c r="AE6"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -3612,7 +3606,7 @@
       <c r="AD7"/>
       <c r="AE7"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3662,7 +3656,7 @@
       <c r="AD8"/>
       <c r="AE8"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -3686,7 +3680,7 @@
       <c r="AD9"/>
       <c r="AE9"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -3727,7 +3721,7 @@
       <c r="AD10"/>
       <c r="AE10"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -3750,7 +3744,7 @@
       <c r="AD11"/>
       <c r="AE11"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -3773,7 +3767,7 @@
       <c r="AD12"/>
       <c r="AE12"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -3847,7 +3841,7 @@
       <c r="AD13"/>
       <c r="AE13"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -3871,7 +3865,7 @@
       <c r="AD14"/>
       <c r="AE14"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -3897,7 +3891,7 @@
       <c r="AD15"/>
       <c r="AE15"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -3923,7 +3917,7 @@
       <c r="AD16"/>
       <c r="AE16"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -3947,7 +3941,7 @@
       <c r="AD17"/>
       <c r="AE17"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -3988,7 +3982,7 @@
       <c r="AD18"/>
       <c r="AE18"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -4011,7 +4005,7 @@
       <c r="AD19"/>
       <c r="AE19"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
@@ -4035,7 +4029,7 @@
       <c r="AD20"/>
       <c r="AE20"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -4085,7 +4079,7 @@
       <c r="AD21"/>
       <c r="AE21"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -4150,7 +4144,7 @@
       <c r="AD22"/>
       <c r="AE22"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -4179,7 +4173,7 @@
       <c r="AD23"/>
       <c r="AE23"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
@@ -4205,7 +4199,7 @@
       <c r="AD24"/>
       <c r="AE24"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
@@ -4294,7 +4288,7 @@
       <c r="AD25"/>
       <c r="AE25"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
@@ -4323,7 +4317,7 @@
       <c r="AD26"/>
       <c r="AE26"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -4352,7 +4346,7 @@
       <c r="AD27"/>
       <c r="AE27"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -4393,7 +4387,7 @@
       <c r="AD28"/>
       <c r="AE28"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -4437,7 +4431,7 @@
       <c r="AD29"/>
       <c r="AE29"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -4466,7 +4460,7 @@
       <c r="AD30"/>
       <c r="AE30"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -4510,7 +4504,7 @@
       <c r="AD31"/>
       <c r="AE31"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -4587,7 +4581,7 @@
       <c r="AD32"/>
       <c r="AE32"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -4655,7 +4649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6728338-95B8-F24D-8833-1C211FF8957D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4663,18 +4657,18 @@
       <selection pane="topRight" activeCell="Y21" sqref="Y21:Z33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4695,7 +4689,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4719,7 +4713,7 @@
         <v>3.6085093400000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4749,7 +4743,7 @@
         <v>3.29245817E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -4770,7 +4764,7 @@
         <v>3.7791573900000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4806,7 +4800,7 @@
         <v>3.3774418099999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4830,7 +4824,7 @@
         <v>3.0433940900000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4854,7 +4848,7 @@
         <v>3.1005594200000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4875,7 +4869,7 @@
         <v>2.5569548700000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4896,7 +4890,7 @@
         <v>3.5006068499999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4923,7 +4917,7 @@
         <v>3.2567766399999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4947,7 +4941,7 @@
         <v>3.7632433900000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -4968,7 +4962,7 @@
         <v>3.4460420400000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5043,7 +5037,7 @@
         <v>15.9795146</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -5082,7 +5076,7 @@
         <v>3.20138787E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -5115,7 +5109,7 @@
         <v>3.2926572000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -5139,7 +5133,7 @@
         <v>4.0493252700000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -5166,7 +5160,7 @@
         <v>3.2121698899999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -5208,7 +5202,7 @@
         <v>3.11629345E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -5229,7 +5223,7 @@
         <v>2.9227657899999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -5250,7 +5244,7 @@
         <v>4.3754093399999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -5298,7 +5292,7 @@
         <v>3.5615801299999999E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -5358,7 +5352,7 @@
         <v>3.7377398699999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -5379,7 +5373,7 @@
         <v>3.3524223099999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -5400,7 +5394,7 @@
         <v>3.4272284699999999E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -5475,7 +5469,7 @@
         <v>2.63216719E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -5496,7 +5490,7 @@
         <v>3.2338318999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -5517,7 +5511,7 @@
         <v>3.5112151899999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -5544,7 +5538,7 @@
         <v>3.37346249E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5565,7 +5559,7 @@
         <v>3.73004554E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -5586,7 +5580,7 @@
         <v>3.4372675800000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -5637,7 +5631,7 @@
         <v>3.3444172999999998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -5718,7 +5712,7 @@
         <v>7.3036754000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -5757,24 +5751,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4375684A-D9A9-674C-932D-4388EBCF0B21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U125"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -5803,7 +5797,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5838,7 +5832,7 @@
         <v>33.080277699999996</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5873,7 +5867,7 @@
         <v>32.290341900000001</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -5908,7 +5902,7 @@
         <v>30.721864500000002</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5943,7 +5937,7 @@
         <v>35.793772699999998</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5981,7 +5975,7 @@
       <c r="S6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -6016,7 +6010,7 @@
         <v>32.824848799999998</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -6051,7 +6045,7 @@
         <v>56.219740000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -6086,7 +6080,7 @@
         <v>32.594371899999999</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -6121,7 +6115,7 @@
         <v>33.110923399999997</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -6156,7 +6150,7 @@
         <v>46.742823600000001</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -6191,7 +6185,7 @@
         <v>33.660075800000001</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -6226,7 +6220,7 @@
         <v>33.288063799999996</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -6261,7 +6255,7 @@
         <v>34.756525699999997</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -6296,7 +6290,7 @@
         <v>33.644091000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -6331,7 +6325,7 @@
         <v>31.3547932</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -6366,7 +6360,7 @@
         <v>30.993404900000002</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -6401,7 +6395,7 @@
         <v>33.425866200000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -6436,7 +6430,7 @@
         <v>30.658167200000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -6471,7 +6465,7 @@
         <v>32.9427254</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -6506,7 +6500,7 @@
         <v>37.530946700000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -6541,7 +6535,7 @@
         <v>30.481838100000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -6576,7 +6570,7 @@
         <v>33.8797383</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -6611,7 +6605,7 @@
         <v>32.858989200000003</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6646,7 +6640,7 @@
         <v>33.924032799999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6681,7 +6675,7 @@
         <v>31.676248600000001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -6716,7 +6710,7 @@
         <v>37.912537700000001</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -6751,7 +6745,7 @@
         <v>37.355130899999999</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -6786,7 +6780,7 @@
         <v>36.922170999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -6821,7 +6815,7 @@
         <v>35.980866599999999</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -6856,7 +6850,7 @@
         <v>32.5294776</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -6891,7 +6885,7 @@
         <v>36.104823199999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -6926,7 +6920,7 @@
         <v>35.545942500000002</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -6961,7 +6955,7 @@
         <v>38.647081100000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -6996,7 +6990,7 @@
         <v>34.469113800000002</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -7031,7 +7025,7 @@
         <v>37.129268500000002</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -7066,7 +7060,7 @@
         <v>32.421107599999999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -7101,7 +7095,7 @@
         <v>34.748995600000001</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -7136,7 +7130,7 @@
         <v>31.672207</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -7171,7 +7165,7 @@
         <v>33.741810199999996</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -7206,7 +7200,7 @@
         <v>38.146359699999998</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -7241,7 +7235,7 @@
         <v>28.2234987</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -7276,7 +7270,7 @@
         <v>35.499110100000003</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -7311,7 +7305,7 @@
         <v>30.1698138</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -7346,7 +7340,7 @@
         <v>31.6049881</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -7381,7 +7375,7 @@
         <v>36.096544700000003</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -7416,7 +7410,7 @@
         <v>34.217773000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -7451,7 +7445,7 @@
         <v>38.1998064</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -7486,7 +7480,7 @@
         <v>38.1998064</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -7521,7 +7515,7 @@
         <v>73.785863000000006</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>21</v>
       </c>
@@ -7556,7 +7550,7 @@
         <v>42.373481199999993</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -7591,7 +7585,7 @@
         <v>37.726657099999997</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -7626,7 +7620,7 @@
         <v>47.270286900000002</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -7661,7 +7655,7 @@
         <v>27.3131506</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -7696,7 +7690,7 @@
         <v>34.544654800000004</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -7731,7 +7725,7 @@
         <v>33.594104700000003</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -7766,7 +7760,7 @@
         <v>34.127969400000005</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -7801,7 +7795,7 @@
         <v>35.813558999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>35</v>
       </c>
@@ -7836,7 +7830,7 @@
         <v>35.056084900000002</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -7871,7 +7865,7 @@
         <v>36.492347699999996</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>30</v>
       </c>
@@ -7906,7 +7900,7 @@
         <v>34.4127796</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -7941,7 +7935,7 @@
         <v>45.281759600000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>32</v>
       </c>
@@ -7976,7 +7970,7 @@
         <v>33.269028200000001</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -8011,7 +8005,7 @@
         <v>31.5234132</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -8046,7 +8040,7 @@
         <v>33.718511999999997</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -8081,7 +8075,7 @@
         <v>33.143779799999997</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -8116,7 +8110,7 @@
         <v>36.9920732</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -8151,7 +8145,7 @@
         <v>33.0499005</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -8186,7 +8180,7 @@
         <v>36.170348599999997</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -8221,7 +8215,7 @@
         <v>27.618890199999999</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -8256,7 +8250,7 @@
         <v>34.6265109</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -8291,7 +8285,7 @@
         <v>34.231739499999996</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -8325,7 +8319,7 @@
         <v>35.1111991</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -8360,7 +8354,7 @@
         <v>32.990459399999999</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -8395,7 +8389,7 @@
         <v>30.166518700000001</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -8430,7 +8424,7 @@
         <v>31.1344776</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -8465,7 +8459,7 @@
         <v>32.381310900000003</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -8500,7 +8494,7 @@
         <v>33.055532499999998</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -8535,7 +8529,7 @@
         <v>37.867810999999996</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -8570,7 +8564,7 @@
         <v>36.3315883</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -8605,7 +8599,7 @@
         <v>34.3600931</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -8640,7 +8634,7 @@
         <v>40.555515299999996</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>22</v>
       </c>
@@ -8675,7 +8669,7 @@
         <v>38.304324299999998</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -8710,7 +8704,7 @@
         <v>33.3007645</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -8745,7 +8739,7 @@
         <v>30.237619599999999</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>25</v>
       </c>
@@ -8780,7 +8774,7 @@
         <v>34.818589299999999</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -8815,7 +8809,7 @@
         <v>40.047744899999998</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -8850,7 +8844,7 @@
         <v>32.569904399999999</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -8885,7 +8879,7 @@
         <v>36.156493600000005</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>35</v>
       </c>
@@ -8920,7 +8914,7 @@
         <v>30.734945900000003</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>29</v>
       </c>
@@ -8955,7 +8949,7 @@
         <v>34.248924899999999</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -8990,7 +8984,7 @@
         <v>34.271445499999999</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>31</v>
       </c>
@@ -9025,7 +9019,7 @@
         <v>40.414650999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>32</v>
       </c>
@@ -9060,7 +9054,7 @@
         <v>35.378555800000001</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>'12.17.18'!A2</f>
         <v>MCAV51</v>
@@ -9096,7 +9090,7 @@
         <v>36.085093399999998</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f>'12.17.18'!A3</f>
         <v>MCAV55</v>
@@ -9132,7 +9126,7 @@
         <v>32.924581699999997</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>'12.17.18'!A4</f>
         <v>MCAV56</v>
@@ -9168,7 +9162,7 @@
         <v>37.791573900000003</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>'12.17.18'!A5</f>
         <v>MCAV58</v>
@@ -9204,7 +9198,7 @@
         <v>33.774418099999998</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>'12.17.18'!A6</f>
         <v>MCAV59</v>
@@ -9240,7 +9234,7 @@
         <v>30.4339409</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>'12.17.18'!A7</f>
         <v>MCAV63</v>
@@ -9276,7 +9270,7 @@
         <v>31.005594200000001</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
         <f>'12.17.18'!A8</f>
         <v>MCAV64</v>
@@ -9312,7 +9306,7 @@
         <v>25.569548700000002</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
         <f>'12.17.18'!A9</f>
         <v>MCAV65</v>
@@ -9348,7 +9342,7 @@
         <v>35.006068499999998</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>'12.17.18'!A10</f>
         <v>MCAV67</v>
@@ -9384,7 +9378,7 @@
         <v>32.567766399999996</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
         <f>'12.17.18'!A11</f>
         <v>MCAV70</v>
@@ -9420,7 +9414,7 @@
         <v>37.632433900000002</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>'12.17.18'!A12</f>
         <v>MCAV75</v>
@@ -9456,7 +9450,7 @@
         <v>34.460420400000004</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>'12.17.18'!A13</f>
         <v>MCAV161</v>
@@ -9492,7 +9486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>'12.17.18'!A14</f>
         <v>MCAV164</v>
@@ -9528,7 +9522,7 @@
         <v>32.013878699999999</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>'12.17.18'!A15</f>
         <v>MCAV165</v>
@@ -9564,7 +9558,7 @@
         <v>32.926572</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
         <f>'12.17.18'!A16</f>
         <v>MCAV166</v>
@@ -9600,7 +9594,7 @@
         <v>40.493252699999999</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>'12.17.18'!A17</f>
         <v>MCAV167</v>
@@ -9636,7 +9630,7 @@
         <v>32.121698899999998</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
         <f>'12.17.18'!A18</f>
         <v>MCAV168</v>
@@ -9672,7 +9666,7 @@
         <v>31.162934499999999</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f>'12.17.18'!A19</f>
         <v>MCAV170</v>
@@ -9708,7 +9702,7 @@
         <v>29.227657899999997</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f>'12.17.18'!A21</f>
         <v>MCAV172</v>
@@ -9744,7 +9738,7 @@
         <v>35.615801300000001</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f>'12.17.18'!A22</f>
         <v>MCAV173</v>
@@ -9780,7 +9774,7 @@
         <v>37.377398700000001</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>'12.17.18'!A23</f>
         <v>MCAV174</v>
@@ -9816,7 +9810,7 @@
         <v>33.5242231</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
         <f>'12.17.18'!A24</f>
         <v>MCAV175</v>
@@ -9852,7 +9846,7 @@
         <v>34.2722847</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
         <f>'12.17.18'!A25</f>
         <v>MCAV181</v>
@@ -9888,7 +9882,7 @@
         <v>26.321671900000002</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f>'12.17.18'!A26</f>
         <v>MCAV182</v>
@@ -9924,7 +9918,7 @@
         <v>32.338318999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f>'12.17.18'!A27</f>
         <v>MCAV183</v>
@@ -9960,7 +9954,7 @@
         <v>35.112151900000001</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f>'12.17.18'!A28</f>
         <v>MCAV184</v>
@@ -9996,7 +9990,7 @@
         <v>33.7346249</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f>'12.17.18'!A29</f>
         <v>MCAV185</v>
@@ -10032,7 +10026,7 @@
         <v>37.300455399999997</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f>'12.17.18'!A30</f>
         <v>MCAV186</v>
@@ -10068,7 +10062,7 @@
         <v>34.372675800000003</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f>'12.17.18'!A31</f>
         <v>MCAV195</v>
@@ -10104,7 +10098,7 @@
         <v>33.444172999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f>'12.17.18'!A32</f>
         <v>MCAV196</v>
@@ -10140,7 +10134,7 @@
         <v>73.036754000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
         <f>'12.17.18'!A33</f>
         <v>MCAV199</v>
@@ -10182,32 +10176,32 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE137F7-C329-6B47-89C5-8391D2285269}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="12.1640625" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" customWidth="1"/>
-    <col min="19" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" customWidth="1"/>
-    <col min="23" max="23" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12.125" customWidth="1"/>
+    <col min="15" max="15" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" customWidth="1"/>
+    <col min="19" max="21" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" customWidth="1"/>
+    <col min="23" max="23" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -10287,7 +10281,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'8.24.18'!A2</f>
         <v>MCAV51</v>
@@ -10398,7 +10392,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'8.24.18'!A3</f>
         <v>MCAV55</v>
@@ -10509,7 +10503,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'8.24.18'!A4</f>
         <v>MCAV56</v>
@@ -10620,7 +10614,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'8.24.18'!A5</f>
         <v>MCAV58</v>
@@ -10731,7 +10725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'8.24.18'!A6</f>
         <v>MCAV59</v>
@@ -10839,7 +10833,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'8.24.18'!A7</f>
         <v>MCAV63</v>
@@ -10947,7 +10941,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'8.24.18'!A8</f>
         <v>MCAV64</v>
@@ -11055,7 +11049,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'8.24.18'!A9</f>
         <v>MCAV65</v>
@@ -11163,7 +11157,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'8.24.18'!A10</f>
         <v>MCAV67</v>
@@ -11271,7 +11265,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'8.24.18'!A11</f>
         <v>MCAV70</v>
@@ -11379,7 +11373,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>'8.24.18'!A12</f>
         <v>MCAV75</v>
@@ -11484,7 +11478,7 @@
         <v>5.266977229730907E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>'8.24.18'!A13</f>
         <v>MCAV161</v>
@@ -11589,7 +11583,7 @@
         <v>0.24855545319865924</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>'8.24.18'!A14</f>
         <v>MCAV164</v>
@@ -11694,7 +11688,7 @@
         <v>0.11359646624578235</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>'8.24.18'!A15</f>
         <v>MCAV165</v>
@@ -11799,7 +11793,7 @@
         <v>0.1139580104517135</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>'8.24.18'!A16</f>
         <v>MCAV166</v>
@@ -11904,7 +11898,7 @@
         <v>0.11980221138914837</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>'8.24.18'!A17</f>
         <v>MCAV167</v>
@@ -12009,7 +12003,7 @@
         <v>-0.12402478333025924</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>'8.24.18'!A18</f>
         <v>MCAV168</v>
@@ -12114,7 +12108,7 @@
         <v>0.17723690271555914</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>'8.24.18'!A19</f>
         <v>MCAV170</v>
@@ -12219,7 +12213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>'8.24.18'!A20</f>
         <v>MCAV172</v>
@@ -12324,7 +12318,7 @@
         <v>0.48795562964107764</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>'8.24.18'!A21</f>
         <v>MCAV173</v>
@@ -12429,7 +12423,7 @@
         <v>0.54645803845312679</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>'8.24.18'!A22</f>
         <v>MCAV174</v>
@@ -12534,7 +12528,7 @@
         <v>2.0341396586207927E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>'8.24.18'!A23</f>
         <v>MCAV175</v>
@@ -12639,7 +12633,7 @@
         <v>-9.5273206308689851E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>'8.24.18'!A24</f>
         <v>MCAV181</v>
@@ -12744,7 +12738,7 @@
         <v>0.45297069859394268</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>'8.24.18'!A25</f>
         <v>MCAV182</v>
@@ -12849,7 +12843,7 @@
         <v>7.7808988284462255E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>'8.24.18'!A26</f>
         <v>MCAV183</v>
@@ -12954,7 +12948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>'8.24.18'!A27</f>
         <v>MCAV184</v>
@@ -13059,7 +13053,7 @@
         <v>0.70107565501773816</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>'8.24.18'!A28</f>
         <v>MCAV185</v>
@@ -13164,7 +13158,7 @@
         <v>0.13047702126621841</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>'8.24.18'!A29</f>
         <v>MCAV186</v>
@@ -13269,7 +13263,7 @@
         <v>7.3722781235799228E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>'8.24.18'!A30</f>
         <v>MCAV195</v>
@@ -13374,7 +13368,7 @@
         <v>0.5220341883159807</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>'8.24.18'!A31</f>
         <v>MCAV196</v>
@@ -13479,7 +13473,7 @@
         <v>0.15436330304267964</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>'8.24.18'!A32</f>
         <v>MCAV199</v>
@@ -13590,29 +13584,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED074980-8C92-B546-88AD-FE439DBE0257}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="12.1640625" customWidth="1"/>
-    <col min="15" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12.125" customWidth="1"/>
+    <col min="15" max="16" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -13758,7 +13752,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'8.24.18'!A2</f>
         <v>MCAV51</v>
@@ -13935,7 +13929,7 @@
         <v>0.45933629247786462</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'8.24.18'!A3</f>
         <v>MCAV55</v>
@@ -14112,7 +14106,7 @@
         <v>5.9516883457209282</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'8.24.18'!A4</f>
         <v>MCAV56</v>
@@ -14289,7 +14283,7 @@
         <v>6.8474213980970919</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'8.24.18'!A5</f>
         <v>MCAV58</v>
@@ -14466,7 +14460,7 @@
         <v>-26.126583300876117</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>'8.24.18'!A6</f>
         <v>MCAV59</v>
@@ -14643,7 +14637,7 @@
         <v>-57.952292319925029</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>'8.24.18'!A7</f>
         <v>MCAV63</v>
@@ -14820,7 +14814,7 @@
         <v>-45.54331760427754</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'8.24.18'!A8</f>
         <v>MCAV64</v>
@@ -14997,7 +14991,7 @@
         <v>-9.3133629965736073</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'8.24.18'!A9</f>
         <v>MCAV65</v>
@@ -15174,7 +15168,7 @@
         <v>-3.8222874558237256</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'8.24.18'!A10</f>
         <v>MCAV67</v>
@@ -15351,7 +15345,7 @@
         <v>-196.35502249871215</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'8.24.18'!A11</f>
         <v>MCAV70</v>
@@ -15528,7 +15522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>'8.24.18'!A12</f>
         <v>MCAV75</v>
@@ -15705,7 +15699,7 @@
         <v>6.1232609940356335</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>'8.24.18'!A13</f>
         <v>MCAV161</v>
@@ -15882,7 +15876,7 @@
         <v>-315.63022419737854</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>'8.24.18'!A14</f>
         <v>MCAV164</v>
@@ -16059,7 +16053,7 @@
         <v>-249.27099505871919</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>'8.24.18'!A15</f>
         <v>MCAV165</v>
@@ -16236,7 +16230,7 @@
         <v>-0.71925520019095468</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>'8.24.18'!A16</f>
         <v>MCAV166</v>
@@ -16413,7 +16407,7 @@
         <v>-9.5243267886341485</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>'8.24.18'!A17</f>
         <v>MCAV167</v>
@@ -16590,7 +16584,7 @@
         <v>-139.38852323371194</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>'8.24.18'!A18</f>
         <v>MCAV168</v>
@@ -16767,7 +16761,7 @@
         <v>-19.859102779717244</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>'8.24.18'!A19</f>
         <v>MCAV170</v>
@@ -16944,7 +16938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>'8.24.18'!A20</f>
         <v>MCAV172</v>
@@ -17121,7 +17115,7 @@
         <v>-143.03783588773436</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>'8.24.18'!A21</f>
         <v>MCAV173</v>
@@ -17298,7 +17292,7 @@
         <v>-34.661927009762302</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>'8.24.18'!A22</f>
         <v>MCAV174</v>
@@ -17475,7 +17469,7 @@
         <v>-13.363610419587115</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>'8.24.18'!A23</f>
         <v>MCAV175</v>
@@ -17652,7 +17646,7 @@
         <v>108.63348368372215</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>'8.24.18'!A24</f>
         <v>MCAV181</v>
@@ -17829,7 +17823,7 @@
         <v>-284.81409440664248</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>'8.24.18'!A25</f>
         <v>MCAV182</v>
@@ -18006,7 +18000,7 @@
         <v>1.0583494722179774</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>'8.24.18'!A26</f>
         <v>MCAV183</v>
@@ -18183,7 +18177,7 @@
         <v>-22.707218434046553</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>'8.24.18'!A27</f>
         <v>MCAV184</v>
@@ -18360,7 +18354,7 @@
         <v>-20.638917297713508</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>'8.24.18'!A28</f>
         <v>MCAV185</v>
@@ -18537,7 +18531,7 @@
         <v>4.7505433972965374</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>'8.24.18'!A29</f>
         <v>MCAV186</v>
@@ -18714,7 +18708,7 @@
         <v>8.6447716295456569</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>'8.24.18'!A30</f>
         <v>MCAV195</v>
@@ -18891,7 +18885,7 @@
         <v>-30.751707909818489</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>'8.24.18'!A31</f>
         <v>MCAV196</v>
@@ -19068,7 +19062,7 @@
         <v>-82.945597449846971</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>'8.24.18'!A32</f>
         <v>MCAV199</v>

</xml_diff>